<commit_message>
rk to commit changes done for login validation"
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>verify &amp; validate that application is checking valid and invalid email format while forgot password the kirana bazaar application.</t>
+  </si>
+  <si>
+    <t>Validate_EmailSentToUser_WhileForgotPassword</t>
+  </si>
+  <si>
+    <t>Verify that email has been sent to user when user name is valid and existing while reset password.</t>
+  </si>
+  <si>
+    <t>Validate_SuccessfulLogin</t>
+  </si>
+  <si>
+    <t>Verif successful login when email and password is valid and existing in database of kirana bazaar.</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,6 +586,34 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Menu Items of Kirana Bazaar and Clicks"
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Verif successful login when email and password is valid and existing in database of kirana bazaar.</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Verif successful navigation to different menu items available in kirana Bazaar application.</t>
+  </si>
+  <si>
+    <t>Navigate_AllMenuItems</t>
   </si>
 </sst>
 </file>
@@ -444,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,10 +619,24 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial commit for positive and negative search
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Verify that application should be shared with whatsap application.</t>
+  </si>
+  <si>
+    <t>Positive_Negative_Search</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Verify that user is able to perform positive and negative search of product in Kirana Bazaar.</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,6 +666,20 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validate pin code scenario !!
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="17430" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17436" windowHeight="5388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Verify that application should be shared with whatsap application.</t>
+  </si>
+  <si>
+    <t>Validate_validPinCodeAtRegistrationPage</t>
+  </si>
+  <si>
+    <t>verify &amp; validate that application is checking valid and invalid pin code format in registration page.</t>
   </si>
 </sst>
 </file>
@@ -459,19 +465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -491,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="28.8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -505,7 +511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="28.8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -519,7 +525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5" ht="28.8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -533,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -547,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -561,7 +567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -589,7 +595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="28.8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -603,7 +609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="28.8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -617,7 +623,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="28.8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -631,7 +637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="28.8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -657,6 +663,20 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.8">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +691,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -683,7 +703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete code for validation scenario
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -132,10 +132,14 @@
     <t>Validate_validPinCodeAtRegistrationPage</t>
   </si>
   <si>
-    <t>verify &amp; validate that application is checking valid and invalid pin code format in registration page.</t>
-  </si>
-  <si>
     <t>Share</t>
+  </si>
+  <si>
+    <t>verify &amp; validate that application is checking the below mentioned points;
+- valid and invalid pin code format in registration page.
+- length allowed for zipcode field.
+- Fetching dynamic zipcodes from Postal APi.
+- Parsing one by one into address fields.</t>
   </si>
 </sst>
 </file>
@@ -479,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -671,13 +675,13 @@
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="90">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -688,7 +692,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">

</xml_diff>

<commit_message>
Test Case Updated in Excel sheet
</commit_message>
<xml_diff>
--- a/app/src/test/java/excelSupport/TestData.xlsx
+++ b/app/src/test/java/excelSupport/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -140,6 +140,24 @@
 - length allowed for zipcode field.
 - Fetching dynamic zipcodes from Postal APi.
 - Parsing one by one into address fields.</t>
+  </si>
+  <si>
+    <t>Verify the max length allowed at each editText available at Kirana Bazaar registration activity</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Verify the max length allowed at feedback editText available at Kirana Bazaar and validate the succesful submission of feedback.</t>
+  </si>
+  <si>
+    <t>Validate_Registration_Maxlength</t>
+  </si>
+  <si>
+    <t>Validate_Feedback</t>
   </si>
 </sst>
 </file>
@@ -481,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -707,6 +725,34 @@
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>